<commit_message>
Rudimentary model using AutoClassifier
</commit_message>
<xml_diff>
--- a/notebooks/EA.xlsx
+++ b/notebooks/EA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Insight\no_more_backlogs\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A3F389C-EC64-4BBC-9281-DC5893709E66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC00494-CFD5-4967-B1C6-51FB084D6F52}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19110" windowHeight="11760"/>
+    <workbookView minimized="1" xWindow="3105" yWindow="5520" windowWidth="9900" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EA" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Chart2" sheetId="3" r:id="rId2"/>
+    <sheet name="EA" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -42,11 +44,20 @@
   <si>
     <t>Volume</t>
   </si>
+  <si>
+    <t>Heirarchichal modeling - for data layers</t>
+  </si>
+  <si>
+    <t>Online game</t>
+  </si>
+  <si>
+    <t>Single player game</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,8 +631,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>EA Anthem</a:t>
+              <a:t>EA </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Opening Security Valuation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -687,6 +705,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:ln w="50800">
+                  <a:solidFill>
+                    <a:srgbClr val="C00000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-F22C-4D8E-ACA1-FFF87AD98A28}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>EA!$A$2:$A$15</c:f>
@@ -792,7 +834,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D455-4960-B97E-13E4CF609450}"/>
+              <c16:uniqueId val="{00000001-F22C-4D8E-ACA1-FFF87AD98A28}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -975,11 +1017,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1018,8 +1056,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Take Two RDR2</a:t>
+              <a:t>Take Two Opening</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Security Valuation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1085,6 +1128,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="50800">
+                  <a:solidFill>
+                    <a:srgbClr val="C00000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-F30A-463A-918C-A6817B2A6C02}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>EA!$K$2:$K$20</c:f>
@@ -1220,7 +1287,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E6F3-4F41-8788-46BFBD047BAB}"/>
+              <c16:uniqueId val="{00000001-F30A-463A-918C-A6817B2A6C02}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1403,11 +1470,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2523,31 +2586,45 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EB7AF0EE-1430-4852-976E-1649692FC3B7}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{67D710FC-F982-4821-95A8-30627FA0A3DB}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9314564" cy="6091570"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{036A17C7-4246-43BB-B3CC-1A153F5CB7AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6F0ADF4-98F8-43A3-8B6D-1A50B45EA803}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2560,30 +2637,73 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.42292</cdr:x>
+      <cdr:y>0.22917</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.62292</cdr:x>
+      <cdr:y>0.5625</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{606E0279-F8D4-403B-8EAA-3F35098B5C34}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1933575" y="628650"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Anthem - Pre-release</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9314564" cy="6091570"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D171CABC-1182-4A9A-8014-FB97C1775E75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18CB54C8-480F-4DF8-A7BC-56B5681F352F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2591,13 +2711,59 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53125</cdr:x>
+      <cdr:y>0.65278</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.73125</cdr:x>
+      <cdr:y>0.98611</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090CA503-FCBD-4FC4-8BB0-8674936AFBB7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2428875" y="1790700"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>RDR2 release</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2896,11 +3062,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,8 +3846,22 @@
         <v>1571300</v>
       </c>
     </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>